<commit_message>
updating test files, examples and excel template. Updating date on dhs_collect.
</commit_message>
<xml_diff>
--- a/src/tests/test_excel-1.xlsx
+++ b/src/tests/test_excel-1.xlsx
@@ -10450,7 +10450,7 @@
       <c r="CF99" s="27" t="inlineStr"/>
     </row>
   </sheetData>
-  <dataValidations count="5">
+  <dataValidations count="6">
     <dataValidation sqref="AB2:AB100 AC2:AC100 AO2:AO100 AR2:AR100 BG2:BG100 BH2:BH100 BI2:BI100 BJ2:BJ100 BK2:BK100 BL2:BL100 BM2:BM100 BN2:BN100 BO2:BO100 BP2:BP100 BQ2:BQ100 BR2:BR100 BS2:BS100 BT2:BT100 BU2:BU100 BV2:BV100 BW2:BW100 BX2:BX100 BZ2:BZ100 CA2:CA100 CB2:CB100 CC2:CC100" showErrorMessage="1" showInputMessage="1" allowBlank="1" errorTitle="Invalid Value" error="Please select true or false, or leave blank." promptTitle="List Selection" prompt="Please select from the list" type="list">
       <formula1>"true,false"</formula1>
     </dataValidation>
@@ -10464,6 +10464,9 @@
     <dataValidation sqref="AA2:AA100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be a number between 1 and 100" type="whole" operator="lessThan">
       <formula1>101</formula1>
     </dataValidation>
+    <dataValidation sqref="A2:A100" showErrorMessage="1" showInputMessage="1" allowBlank="0" errorTitle="Invalid Entry" error="This value must be string with no spaces and a max of 128 chars" type="custom">
+      <formula1>AND(LEN(A2)&lt;129,NOT(ISNUMBER(SEARCH(" ",A2))))</formula1>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <legacyDrawing xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="anysvml"/>

</xml_diff>